<commit_message>
Fusão da InicializaSolver e fim da CalcLimite
1. Foi criada uma função para disponibilizar as funções simbólicas na área de trabalho.
2. Não existe mais a CalcLimites. Ela foi inserida na função que cria a tabela de limites dinâmicos. Ninguém mais a consome. Aproveitei para colocar TUDO na mesma ordem que consumimos, padronizando isso, ou seja, a reorganização foi feita na criação da tabela e a tabela/matriz terá formato único e ordem única para ser consumida por todos
3. Foi adaptada a CalcLimitesSym (para o Simulink) para usar da função simbólica (já na mesma ordem)
4. No Simulink, foi ajustado o Bloco que faz as contas de restrições dinâmicas (mas só o CBR vai consumir). Inclusive foram extraídas variáveis que não usamos e as variáveis já estão na mesma ordem.
5 - Não existe mais a InicializaSolver, ela foi fundida com a CasadiBlock.
</commit_message>
<xml_diff>
--- a/Tabelas/TabelaLimitesDinamicos.xlsx
+++ b/Tabelas/TabelaLimitesDinamicos.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>Frequencia</t>
   </si>
@@ -230,6 +230,42 @@
   <si>
     <t>VazaoOleo</t>
   </si>
+  <si>
+    <t>Frequencia</t>
+  </si>
+  <si>
+    <t>PSuc</t>
+  </si>
+  <si>
+    <t>PChegada</t>
+  </si>
+  <si>
+    <t>PDiff</t>
+  </si>
+  <si>
+    <t>PDescarga</t>
+  </si>
+  <si>
+    <t>TMotor</t>
+  </si>
+  <si>
+    <t>ITorque</t>
+  </si>
+  <si>
+    <t>ITotal</t>
+  </si>
+  <si>
+    <t>TSuc</t>
+  </si>
+  <si>
+    <t>Vibracao</t>
+  </si>
+  <si>
+    <t>TChegada</t>
+  </si>
+  <si>
+    <t>VazaoOleo</t>
+  </si>
 </sst>
 </file>
 
@@ -249,7 +285,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -263,11 +299,12 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -275,6 +312,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -288,55 +326,55 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.046875" customWidth="true"/>
-    <col min="2" max="2" width="13.15625" customWidth="true"/>
-    <col min="3" max="3" width="23.046875" customWidth="true"/>
-    <col min="4" max="4" width="17.26953125" customWidth="true"/>
-    <col min="5" max="5" width="15.93359375" customWidth="true"/>
+    <col min="2" max="2" width="11.7109375" customWidth="true"/>
+    <col min="3" max="3" width="11.7109375" customWidth="true"/>
+    <col min="4" max="4" width="5.15625" customWidth="true"/>
+    <col min="5" max="5" width="9.6015625" customWidth="true"/>
     <col min="6" max="6" width="7.37890625" customWidth="true"/>
-    <col min="7" max="7" width="13.046875" customWidth="true"/>
-    <col min="8" max="8" width="11.48828125" customWidth="true"/>
-    <col min="9" max="9" width="4.82421875" customWidth="true"/>
+    <col min="7" max="7" width="7.7109375" customWidth="true"/>
+    <col min="8" max="8" width="5.93359375" customWidth="true"/>
+    <col min="9" max="9" width="4.93359375" customWidth="true"/>
     <col min="10" max="10" width="8.37890625" customWidth="true"/>
-    <col min="11" max="11" width="26.7109375" customWidth="true"/>
+    <col min="11" max="11" width="9.15625" customWidth="true"/>
     <col min="12" max="12" width="10.046875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
atualiza tabelas para melhor resolução
</commit_message>
<xml_diff>
--- a/Tabelas/TabelaLimitesDinamicos.xlsx
+++ b/Tabelas/TabelaLimitesDinamicos.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="168">
   <si>
     <t>Frequencia</t>
   </si>
@@ -226,6 +226,42 @@
   </si>
   <si>
     <t>ProductionSurfaceTemperature</t>
+  </si>
+  <si>
+    <t>VazaoOleo</t>
+  </si>
+  <si>
+    <t>Frequencia</t>
+  </si>
+  <si>
+    <t>PSuc</t>
+  </si>
+  <si>
+    <t>PChegada</t>
+  </si>
+  <si>
+    <t>PDiff</t>
+  </si>
+  <si>
+    <t>PDescarga</t>
+  </si>
+  <si>
+    <t>TMotor</t>
+  </si>
+  <si>
+    <t>ITorque</t>
+  </si>
+  <si>
+    <t>ITotal</t>
+  </si>
+  <si>
+    <t>TSuc</t>
+  </si>
+  <si>
+    <t>Vibracao</t>
+  </si>
+  <si>
+    <t>TChegada</t>
   </si>
   <si>
     <t>VazaoOleo</t>
@@ -501,7 +537,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -522,11 +558,12 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -541,6 +578,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,40 +607,40 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2">
@@ -613,7 +651,7 @@
         <v>110</v>
       </c>
       <c r="C2" s="0">
-        <v>33.34261696393898</v>
+        <v>34.323282168760713</v>
       </c>
       <c r="D2" s="0">
         <v>150</v>
@@ -678,7 +716,7 @@
         <v>40</v>
       </c>
       <c r="L3" s="0">
-        <v>199.5</v>
+        <v>194.04999999999995</v>
       </c>
     </row>
     <row r="4">
@@ -689,7 +727,7 @@
         <v>110</v>
       </c>
       <c r="C4" s="0">
-        <v>33.34261696393898</v>
+        <v>34.323282168760713</v>
       </c>
       <c r="D4" s="0">
         <v>150</v>
@@ -754,7 +792,7 @@
         <v>40</v>
       </c>
       <c r="L5" s="0">
-        <v>201.67000000000007</v>
+        <v>196.27499999999998</v>
       </c>
     </row>
     <row r="6">
@@ -765,7 +803,7 @@
         <v>110</v>
       </c>
       <c r="C6" s="0">
-        <v>33.34261696393898</v>
+        <v>34.813614771171579</v>
       </c>
       <c r="D6" s="0">
         <v>150</v>
@@ -830,7 +868,7 @@
         <v>40</v>
       </c>
       <c r="L7" s="0">
-        <v>203.84000000000003</v>
+        <v>195.83000000000004</v>
       </c>
     </row>
     <row r="8">
@@ -993,7 +1031,7 @@
         <v>110</v>
       </c>
       <c r="C12" s="0">
-        <v>35.303947373582446</v>
+        <v>35.794279975993312</v>
       </c>
       <c r="D12" s="0">
         <v>150</v>
@@ -1058,7 +1096,7 @@
         <v>40</v>
       </c>
       <c r="L13" s="0">
-        <v>200</v>
+        <v>197.28749999999999</v>
       </c>
     </row>
     <row r="14">
@@ -1069,7 +1107,7 @@
         <v>110</v>
       </c>
       <c r="C14" s="0">
-        <v>35.303947373582446</v>
+        <v>36.284612578404179</v>
       </c>
       <c r="D14" s="0">
         <v>150</v>
@@ -1134,7 +1172,7 @@
         <v>40</v>
       </c>
       <c r="L15" s="0">
-        <v>202.28000000000009</v>
+        <v>196.91999999999996</v>
       </c>
     </row>
     <row r="16">
@@ -1145,7 +1183,7 @@
         <v>110</v>
       </c>
       <c r="C16" s="0">
-        <v>35.303947373582446</v>
+        <v>36.284612578404179</v>
       </c>
       <c r="D16" s="0">
         <v>150</v>
@@ -1172,7 +1210,7 @@
         <v>100</v>
       </c>
       <c r="L16" s="0">
-        <v>314.16000000000008</v>
+        <v>314.15999999999997</v>
       </c>
     </row>
     <row r="17">
@@ -1210,7 +1248,7 @@
         <v>40</v>
       </c>
       <c r="L17" s="0">
-        <v>204.56000000000006</v>
+        <v>199.26499999999999</v>
       </c>
     </row>
     <row r="18">
@@ -1221,7 +1259,7 @@
         <v>110</v>
       </c>
       <c r="C18" s="0">
-        <v>35.303947373582446</v>
+        <v>36.774945180815045</v>
       </c>
       <c r="D18" s="0">
         <v>150</v>
@@ -1248,7 +1286,7 @@
         <v>100</v>
       </c>
       <c r="L18" s="0">
-        <v>315.53999999999996</v>
+        <v>315.53999999999985</v>
       </c>
     </row>
     <row r="19">
@@ -1286,7 +1324,7 @@
         <v>40</v>
       </c>
       <c r="L19" s="0">
-        <v>206.83999999999992</v>
+        <v>198.99499999999989</v>
       </c>
     </row>
     <row r="20">
@@ -1449,7 +1487,7 @@
         <v>110</v>
       </c>
       <c r="C24" s="0">
-        <v>37.265277783225912</v>
+        <v>37.755610385636786</v>
       </c>
       <c r="D24" s="0">
         <v>150</v>
@@ -1476,7 +1514,7 @@
         <v>100</v>
       </c>
       <c r="L24" s="0">
-        <v>319.66000000000014</v>
+        <v>319.66000000000003</v>
       </c>
     </row>
     <row r="25">
@@ -1514,7 +1552,7 @@
         <v>40</v>
       </c>
       <c r="L25" s="0">
-        <v>203.40000000000009</v>
+        <v>200.77750000000003</v>
       </c>
     </row>
     <row r="26">
@@ -1525,7 +1563,7 @@
         <v>110</v>
       </c>
       <c r="C26" s="0">
-        <v>37.265277783225912</v>
+        <v>38.245942988047652</v>
       </c>
       <c r="D26" s="0">
         <v>150</v>
@@ -1552,7 +1590,7 @@
         <v>100</v>
       </c>
       <c r="L26" s="0">
-        <v>321.02000000000015</v>
+        <v>321.02000000000004</v>
       </c>
     </row>
     <row r="27">
@@ -1590,7 +1628,7 @@
         <v>40</v>
       </c>
       <c r="L27" s="0">
-        <v>205.60000000000014</v>
+        <v>200.4100000000002</v>
       </c>
     </row>
     <row r="28">
@@ -1601,7 +1639,7 @@
         <v>110</v>
       </c>
       <c r="C28" s="0">
-        <v>37.265277783225912</v>
+        <v>38.736275590458519</v>
       </c>
       <c r="D28" s="0">
         <v>150</v>
@@ -1666,7 +1704,7 @@
         <v>40</v>
       </c>
       <c r="L29" s="0">
-        <v>207.79999999999995</v>
+        <v>200.09749999999997</v>
       </c>
     </row>
     <row r="30">
@@ -1677,7 +1715,7 @@
         <v>110</v>
       </c>
       <c r="C30" s="0">
-        <v>37.265277783225912</v>
+        <v>38.736275590458519</v>
       </c>
       <c r="D30" s="0">
         <v>150</v>
@@ -1742,7 +1780,7 @@
         <v>40</v>
       </c>
       <c r="L31" s="0">
-        <v>210</v>
+        <v>202.38</v>
       </c>
     </row>
     <row r="32">
@@ -1829,7 +1867,7 @@
         <v>110</v>
       </c>
       <c r="C34" s="0">
-        <v>39.226608192869385</v>
+        <v>39.716940795280252</v>
       </c>
       <c r="D34" s="0">
         <v>150</v>
@@ -1894,7 +1932,7 @@
         <v>40</v>
       </c>
       <c r="L35" s="0">
-        <v>204.46000000000004</v>
+        <v>201.82999999999993</v>
       </c>
     </row>
     <row r="36">
@@ -1905,7 +1943,7 @@
         <v>110</v>
       </c>
       <c r="C36" s="0">
-        <v>39.226608192869385</v>
+        <v>39.716940795280252</v>
       </c>
       <c r="D36" s="0">
         <v>150</v>
@@ -1970,7 +2008,7 @@
         <v>40</v>
       </c>
       <c r="L37" s="0">
-        <v>206.7700000000001</v>
+        <v>204.17250000000001</v>
       </c>
     </row>
     <row r="38">
@@ -1981,7 +2019,7 @@
         <v>110</v>
       </c>
       <c r="C38" s="0">
-        <v>39.226608192869385</v>
+        <v>40.207273397691118</v>
       </c>
       <c r="D38" s="0">
         <v>150</v>
@@ -2046,7 +2084,7 @@
         <v>40</v>
       </c>
       <c r="L39" s="0">
-        <v>209.07999999999993</v>
+        <v>203.94999999999993</v>
       </c>
     </row>
     <row r="40">
@@ -2057,7 +2095,7 @@
         <v>110</v>
       </c>
       <c r="C40" s="0">
-        <v>39.226608192869385</v>
+        <v>40.697606000101985</v>
       </c>
       <c r="D40" s="0">
         <v>150</v>
@@ -2122,7 +2160,7 @@
         <v>40</v>
       </c>
       <c r="L41" s="0">
-        <v>211.38999999999999</v>
+        <v>203.79250000000002</v>
       </c>
     </row>
     <row r="42">
@@ -2274,7 +2312,7 @@
         <v>40</v>
       </c>
       <c r="L45" s="0">
-        <v>205.92999999999995</v>
+        <v>205.93000000000006</v>
       </c>
     </row>
     <row r="46">
@@ -2285,7 +2323,7 @@
         <v>110</v>
       </c>
       <c r="C46" s="0">
-        <v>41.187938602512851</v>
+        <v>41.678271204923718</v>
       </c>
       <c r="D46" s="0">
         <v>150</v>
@@ -2350,7 +2388,7 @@
         <v>40</v>
       </c>
       <c r="L47" s="0">
-        <v>208.15999999999997</v>
+        <v>205.61500000000012</v>
       </c>
     </row>
     <row r="48">
@@ -2361,7 +2399,7 @@
         <v>110</v>
       </c>
       <c r="C48" s="0">
-        <v>41.187938602512851</v>
+        <v>42.168603807334591</v>
       </c>
       <c r="D48" s="0">
         <v>150</v>
@@ -2426,7 +2464,7 @@
         <v>40</v>
       </c>
       <c r="L49" s="0">
-        <v>210.38999999999987</v>
+        <v>205.3549999999999</v>
       </c>
     </row>
     <row r="50">
@@ -2437,7 +2475,7 @@
         <v>110</v>
       </c>
       <c r="C50" s="0">
-        <v>41.187938602512851</v>
+        <v>42.168603807334591</v>
       </c>
       <c r="D50" s="0">
         <v>150</v>
@@ -2502,7 +2540,7 @@
         <v>40</v>
       </c>
       <c r="L51" s="0">
-        <v>212.61999999999989</v>
+        <v>207.63999999999999</v>
       </c>
     </row>
     <row r="52">
@@ -2513,7 +2551,7 @@
         <v>110</v>
       </c>
       <c r="C52" s="0">
-        <v>41.187938602512851</v>
+        <v>42.658936409745458</v>
       </c>
       <c r="D52" s="0">
         <v>150</v>
@@ -2578,7 +2616,7 @@
         <v>40</v>
       </c>
       <c r="L53" s="0">
-        <v>214.84999999999991</v>
+        <v>207.46250000000001</v>
       </c>
     </row>
     <row r="54">
@@ -2616,7 +2654,7 @@
         <v>100</v>
       </c>
       <c r="L54" s="0">
-        <v>339.94000000000005</v>
+        <v>339.93999999999994</v>
       </c>
     </row>
     <row r="55">
@@ -2665,7 +2703,7 @@
         <v>110</v>
       </c>
       <c r="C56" s="0">
-        <v>43.149269012156324</v>
+        <v>43.639601614567191</v>
       </c>
       <c r="D56" s="0">
         <v>150</v>
@@ -2692,7 +2730,7 @@
         <v>100</v>
       </c>
       <c r="L56" s="0">
-        <v>341.28000000000009</v>
+        <v>341.27999999999997</v>
       </c>
     </row>
     <row r="57">
@@ -2730,7 +2768,7 @@
         <v>40</v>
       </c>
       <c r="L57" s="0">
-        <v>209.67999999999995</v>
+        <v>207.16500000000008</v>
       </c>
     </row>
     <row r="58">
@@ -2741,7 +2779,7 @@
         <v>110</v>
       </c>
       <c r="C58" s="0">
-        <v>43.149269012156324</v>
+        <v>43.639601614567191</v>
       </c>
       <c r="D58" s="0">
         <v>150</v>
@@ -2768,7 +2806,7 @@
         <v>100</v>
       </c>
       <c r="L58" s="0">
-        <v>342.62</v>
+        <v>342.61999999999989</v>
       </c>
     </row>
     <row r="59">
@@ -2806,7 +2844,7 @@
         <v>40</v>
       </c>
       <c r="L59" s="0">
-        <v>212.01999999999987</v>
+        <v>209.53499999999997</v>
       </c>
     </row>
     <row r="60">
@@ -2817,7 +2855,7 @@
         <v>110</v>
       </c>
       <c r="C60" s="0">
-        <v>43.149269012156324</v>
+        <v>44.129934216978057</v>
       </c>
       <c r="D60" s="0">
         <v>150</v>
@@ -2844,7 +2882,7 @@
         <v>100</v>
       </c>
       <c r="L60" s="0">
-        <v>343.96000000000004</v>
+        <v>343.95999999999992</v>
       </c>
     </row>
     <row r="61">
@@ -2882,7 +2920,7 @@
         <v>40</v>
       </c>
       <c r="L61" s="0">
-        <v>214.3599999999999</v>
+        <v>209.44999999999993</v>
       </c>
     </row>
     <row r="62">
@@ -2893,7 +2931,7 @@
         <v>110</v>
       </c>
       <c r="C62" s="0">
-        <v>43.149269012156324</v>
+        <v>44.620266819388924</v>
       </c>
       <c r="D62" s="0">
         <v>150</v>
@@ -2958,7 +2996,7 @@
         <v>40</v>
       </c>
       <c r="L63" s="0">
-        <v>216.69999999999999</v>
+        <v>209.42500000000001</v>
       </c>
     </row>
     <row r="64">
@@ -2996,7 +3034,7 @@
         <v>100</v>
       </c>
       <c r="L64" s="0">
-        <v>346.62999999999994</v>
+        <v>346.63000000000005</v>
       </c>
     </row>
     <row r="65">
@@ -3072,7 +3110,7 @@
         <v>100</v>
       </c>
       <c r="L66" s="0">
-        <v>347.95999999999998</v>
+        <v>347.96000000000009</v>
       </c>
     </row>
     <row r="67">
@@ -3121,7 +3159,7 @@
         <v>110</v>
       </c>
       <c r="C68" s="0">
-        <v>45.11059942179979</v>
+        <v>45.600932024210657</v>
       </c>
       <c r="D68" s="0">
         <v>150</v>
@@ -3186,7 +3224,7 @@
         <v>40</v>
       </c>
       <c r="L69" s="0">
-        <v>213.74999999999989</v>
+        <v>211.27499999999998</v>
       </c>
     </row>
     <row r="70">
@@ -3197,7 +3235,7 @@
         <v>110</v>
       </c>
       <c r="C70" s="0">
-        <v>45.11059942179979</v>
+        <v>46.091264626621523</v>
       </c>
       <c r="D70" s="0">
         <v>150</v>
@@ -3262,7 +3300,7 @@
         <v>40</v>
       </c>
       <c r="L71" s="0">
-        <v>216</v>
+        <v>211.10000000000002</v>
       </c>
     </row>
     <row r="72">
@@ -3273,7 +3311,7 @@
         <v>110</v>
       </c>
       <c r="C72" s="0">
-        <v>45.11059942179979</v>
+        <v>46.581597229032397</v>
       </c>
       <c r="D72" s="0">
         <v>150</v>
@@ -3338,7 +3376,7 @@
         <v>40</v>
       </c>
       <c r="L73" s="0">
-        <v>218.25</v>
+        <v>210.97500000000002</v>
       </c>
     </row>
     <row r="74">
@@ -3349,7 +3387,7 @@
         <v>110</v>
       </c>
       <c r="C74" s="0">
-        <v>45.11059942179979</v>
+        <v>46.581597229032397</v>
       </c>
       <c r="D74" s="0">
         <v>150</v>
@@ -3414,7 +3452,7 @@
         <v>40</v>
       </c>
       <c r="L75" s="0">
-        <v>220.5</v>
+        <v>213.30000000000007</v>
       </c>
     </row>
     <row r="76">
@@ -3452,7 +3490,7 @@
         <v>100</v>
       </c>
       <c r="L76" s="0">
-        <v>354.60999999999996</v>
+        <v>354.61000000000007</v>
       </c>
     </row>
     <row r="77">
@@ -3501,7 +3539,7 @@
         <v>110</v>
       </c>
       <c r="C78" s="0">
-        <v>47.071929831443263</v>
+        <v>47.56226243385413</v>
       </c>
       <c r="D78" s="0">
         <v>150</v>
@@ -3528,7 +3566,7 @@
         <v>100</v>
       </c>
       <c r="L78" s="0">
-        <v>355.93999999999988</v>
+        <v>355.94</v>
       </c>
     </row>
     <row r="79">
@@ -3566,7 +3604,7 @@
         <v>40</v>
       </c>
       <c r="L79" s="0">
-        <v>215.59999999999991</v>
+        <v>213.19000000000017</v>
       </c>
     </row>
     <row r="80">
@@ -3577,7 +3615,7 @@
         <v>110</v>
       </c>
       <c r="C80" s="0">
-        <v>47.071929831443263</v>
+        <v>48.052595036264997</v>
       </c>
       <c r="D80" s="0">
         <v>150</v>
@@ -3604,7 +3642,7 @@
         <v>100</v>
       </c>
       <c r="L80" s="0">
-        <v>357.26999999999992</v>
+        <v>357.27000000000004</v>
       </c>
     </row>
     <row r="81">
@@ -3642,7 +3680,7 @@
         <v>40</v>
       </c>
       <c r="L81" s="0">
-        <v>217.94999999999982</v>
+        <v>213.18999999999983</v>
       </c>
     </row>
     <row r="82">
@@ -3653,7 +3691,7 @@
         <v>110</v>
       </c>
       <c r="C82" s="0">
-        <v>47.071929831443263</v>
+        <v>48.542927638675863</v>
       </c>
       <c r="D82" s="0">
         <v>150</v>
@@ -3718,7 +3756,7 @@
         <v>40</v>
       </c>
       <c r="L83" s="0">
-        <v>220.30000000000001</v>
+        <v>213.25</v>
       </c>
     </row>
     <row r="84">
@@ -3729,7 +3767,7 @@
         <v>110</v>
       </c>
       <c r="C84" s="0">
-        <v>47.071929831443263</v>
+        <v>48.542927638675863</v>
       </c>
       <c r="D84" s="0">
         <v>150</v>
@@ -3794,7 +3832,7 @@
         <v>40</v>
       </c>
       <c r="L85" s="0">
-        <v>222.48000000000013</v>
+        <v>215.49000000000001</v>
       </c>
     </row>
     <row r="86">
@@ -3870,7 +3908,7 @@
         <v>40</v>
       </c>
       <c r="L87" s="0">
-        <v>215.42000000000007</v>
+        <v>215.41999999999996</v>
       </c>
     </row>
     <row r="88">
@@ -3881,7 +3919,7 @@
         <v>110</v>
       </c>
       <c r="C88" s="0">
-        <v>49.03326024108673</v>
+        <v>49.523592843497596</v>
       </c>
       <c r="D88" s="0">
         <v>150</v>
@@ -3946,7 +3984,7 @@
         <v>40</v>
       </c>
       <c r="L89" s="0">
-        <v>217.67999999999995</v>
+        <v>215.27999999999986</v>
       </c>
     </row>
     <row r="90">
@@ -3957,7 +3995,7 @@
         <v>110</v>
       </c>
       <c r="C90" s="0">
-        <v>49.03326024108673</v>
+        <v>50.013925445908463</v>
       </c>
       <c r="D90" s="0">
         <v>150</v>
@@ -3984,7 +4022,7 @@
         <v>100</v>
       </c>
       <c r="L90" s="0">
-        <v>363.84000000000003</v>
+        <v>363.83999999999992</v>
       </c>
     </row>
     <row r="91">
@@ -4022,7 +4060,7 @@
         <v>40</v>
       </c>
       <c r="L91" s="0">
-        <v>219.93999999999994</v>
+        <v>215.19000000000005</v>
       </c>
     </row>
     <row r="92">
@@ -4033,7 +4071,7 @@
         <v>110</v>
       </c>
       <c r="C92" s="0">
-        <v>49.03326024108673</v>
+        <v>50.013925445908463</v>
       </c>
       <c r="D92" s="0">
         <v>150</v>
@@ -4098,7 +4136,7 @@
         <v>40</v>
       </c>
       <c r="L93" s="0">
-        <v>222.19999999999993</v>
+        <v>217.5</v>
       </c>
     </row>
     <row r="94">
@@ -4109,7 +4147,7 @@
         <v>110</v>
       </c>
       <c r="C94" s="0">
-        <v>49.03326024108673</v>
+        <v>50.504258048319336</v>
       </c>
       <c r="D94" s="0">
         <v>150</v>
@@ -4174,7 +4212,7 @@
         <v>40</v>
       </c>
       <c r="L95" s="0">
-        <v>224.46000000000004</v>
+        <v>217.48500000000001</v>
       </c>
     </row>
     <row r="96">
@@ -4212,7 +4250,7 @@
         <v>100</v>
       </c>
       <c r="L96" s="0">
-        <v>367.76999999999998</v>
+        <v>367.7700000000001</v>
       </c>
     </row>
     <row r="97">
@@ -4261,7 +4299,7 @@
         <v>110</v>
       </c>
       <c r="C98" s="0">
-        <v>50.994590650730203</v>
+        <v>51.484923253141069</v>
       </c>
       <c r="D98" s="0">
         <v>150</v>
@@ -4288,7 +4326,7 @@
         <v>100</v>
       </c>
       <c r="L98" s="0">
-        <v>369.07999999999993</v>
+        <v>369.08000000000004</v>
       </c>
     </row>
     <row r="99">
@@ -4326,7 +4364,7 @@
         <v>40</v>
       </c>
       <c r="L99" s="0">
-        <v>219.88000000000011</v>
+        <v>217.52499999999986</v>
       </c>
     </row>
     <row r="100">
@@ -4337,7 +4375,7 @@
         <v>110</v>
       </c>
       <c r="C100" s="0">
-        <v>50.994590650730203</v>
+        <v>51.975255855551936</v>
       </c>
       <c r="D100" s="0">
         <v>150</v>
@@ -4402,7 +4440,7 @@
         <v>40</v>
       </c>
       <c r="L101" s="0">
-        <v>222.24000000000001</v>
+        <v>217.58500000000004</v>
       </c>
     </row>
     <row r="102">
@@ -4413,7 +4451,7 @@
         <v>110</v>
       </c>
       <c r="C102" s="0">
-        <v>50.994590650730203</v>
+        <v>51.975255855551936</v>
       </c>
       <c r="D102" s="0">
         <v>150</v>
@@ -4478,7 +4516,7 @@
         <v>40</v>
       </c>
       <c r="L103" s="0">
-        <v>224.59999999999999</v>
+        <v>220.00000000000003</v>
       </c>
     </row>
     <row r="104">
@@ -4489,7 +4527,7 @@
         <v>110</v>
       </c>
       <c r="C104" s="0">
-        <v>50.994590650730203</v>
+        <v>52.465588457962802</v>
       </c>
       <c r="D104" s="0">
         <v>150</v>
@@ -4554,7 +4592,7 @@
         <v>40</v>
       </c>
       <c r="L105" s="0">
-        <v>226.79000000000008</v>
+        <v>219.95000000000005</v>
       </c>
     </row>
     <row r="106">
@@ -4641,7 +4679,7 @@
         <v>110</v>
       </c>
       <c r="C108" s="0">
-        <v>52.955921060373669</v>
+        <v>53.446253662784535</v>
       </c>
       <c r="D108" s="0">
         <v>150</v>
@@ -4706,7 +4744,7 @@
         <v>40</v>
       </c>
       <c r="L109" s="0">
-        <v>222.20999999999992</v>
+        <v>219.87749999999983</v>
       </c>
     </row>
     <row r="110">
@@ -4717,7 +4755,7 @@
         <v>110</v>
       </c>
       <c r="C110" s="0">
-        <v>52.955921060373669</v>
+        <v>53.936586265195402</v>
       </c>
       <c r="D110" s="0">
         <v>150</v>
@@ -4782,7 +4820,7 @@
         <v>40</v>
       </c>
       <c r="L111" s="0">
-        <v>224.4799999999999</v>
+        <v>219.8599999999999</v>
       </c>
     </row>
     <row r="112">
@@ -4793,7 +4831,7 @@
         <v>110</v>
       </c>
       <c r="C112" s="0">
-        <v>52.955921060373669</v>
+        <v>53.936586265195402</v>
       </c>
       <c r="D112" s="0">
         <v>150</v>
@@ -4858,7 +4896,7 @@
         <v>40</v>
       </c>
       <c r="L113" s="0">
-        <v>226.74999999999989</v>
+        <v>222.17499999999998</v>
       </c>
     </row>
     <row r="114">
@@ -4869,7 +4907,7 @@
         <v>110</v>
       </c>
       <c r="C114" s="0">
-        <v>52.955921060373669</v>
+        <v>54.426918867606268</v>
       </c>
       <c r="D114" s="0">
         <v>150</v>
@@ -4896,7 +4934,7 @@
         <v>100</v>
       </c>
       <c r="L114" s="0">
-        <v>379.44</v>
+        <v>379.43999999999988</v>
       </c>
     </row>
     <row r="115">
@@ -4934,7 +4972,7 @@
         <v>40</v>
       </c>
       <c r="L115" s="0">
-        <v>229.01999999999987</v>
+        <v>222.22499999999991</v>
       </c>
     </row>
     <row r="116">
@@ -5021,7 +5059,7 @@
         <v>110</v>
       </c>
       <c r="C118" s="0">
-        <v>54.917251470017142</v>
+        <v>55.407584072428008</v>
       </c>
       <c r="D118" s="0">
         <v>150</v>
@@ -5086,7 +5124,7 @@
         <v>40</v>
       </c>
       <c r="L119" s="0">
-        <v>224.67999999999984</v>
+        <v>222.38</v>
       </c>
     </row>
     <row r="120">
@@ -5097,7 +5135,7 @@
         <v>110</v>
       </c>
       <c r="C120" s="0">
-        <v>54.917251470017142</v>
+        <v>55.897916674838875</v>
       </c>
       <c r="D120" s="0">
         <v>150</v>
@@ -5162,7 +5200,7 @@
         <v>40</v>
       </c>
       <c r="L121" s="0">
-        <v>227.03999999999996</v>
+        <v>222.49000000000012</v>
       </c>
     </row>
     <row r="122">
@@ -5173,7 +5211,7 @@
         <v>110</v>
       </c>
       <c r="C122" s="0">
-        <v>54.917251470017142</v>
+        <v>56.388249277249741</v>
       </c>
       <c r="D122" s="0">
         <v>150</v>
@@ -5238,7 +5276,7 @@
         <v>40</v>
       </c>
       <c r="L123" s="0">
-        <v>229.40000000000001</v>
+        <v>222.64999999999998</v>
       </c>
     </row>
     <row r="124">
@@ -5249,7 +5287,7 @@
         <v>110</v>
       </c>
       <c r="C124" s="0">
-        <v>54.917251470017142</v>
+        <v>56.388249277249741</v>
       </c>
       <c r="D124" s="0">
         <v>150</v>
@@ -5314,7 +5352,7 @@
         <v>40</v>
       </c>
       <c r="L125" s="0">
-        <v>231.58999999999992</v>
+        <v>224.89999999999998</v>
       </c>
     </row>
     <row r="126">
@@ -5401,7 +5439,7 @@
         <v>110</v>
       </c>
       <c r="C128" s="0">
-        <v>56.878581879660608</v>
+        <v>57.368914482071474</v>
       </c>
       <c r="D128" s="0">
         <v>150</v>
@@ -5466,7 +5504,7 @@
         <v>40</v>
       </c>
       <c r="L129" s="0">
-        <v>227.20999999999992</v>
+        <v>224.9525000000001</v>
       </c>
     </row>
     <row r="130">
@@ -5477,7 +5515,7 @@
         <v>110</v>
       </c>
       <c r="C130" s="0">
-        <v>56.878581879660608</v>
+        <v>57.859247084482341</v>
       </c>
       <c r="D130" s="0">
         <v>150</v>
@@ -5542,7 +5580,7 @@
         <v>40</v>
       </c>
       <c r="L131" s="0">
-        <v>229.48000000000013</v>
+        <v>225.00999999999999</v>
       </c>
     </row>
     <row r="132">
@@ -5553,7 +5591,7 @@
         <v>110</v>
       </c>
       <c r="C132" s="0">
-        <v>56.878581879660608</v>
+        <v>58.349579686893208</v>
       </c>
       <c r="D132" s="0">
         <v>150</v>
@@ -5618,7 +5656,7 @@
         <v>40</v>
       </c>
       <c r="L133" s="0">
-        <v>231.75000000000011</v>
+        <v>225.11249999999998</v>
       </c>
     </row>
     <row r="134">
@@ -5629,7 +5667,7 @@
         <v>110</v>
       </c>
       <c r="C134" s="0">
-        <v>56.878581879660608</v>
+        <v>58.349579686893208</v>
       </c>
       <c r="D134" s="0">
         <v>150</v>
@@ -5694,7 +5732,7 @@
         <v>40</v>
       </c>
       <c r="L135" s="0">
-        <v>234.0200000000001</v>
+        <v>227.45000000000005</v>
       </c>
     </row>
     <row r="136">
@@ -5770,7 +5808,7 @@
         <v>40</v>
       </c>
       <c r="L137" s="0">
-        <v>227.62000000000023</v>
+        <v>227.62</v>
       </c>
     </row>
     <row r="138">
@@ -5781,7 +5819,7 @@
         <v>110</v>
       </c>
       <c r="C138" s="0">
-        <v>58.839912289304074</v>
+        <v>59.330244891714948</v>
       </c>
       <c r="D138" s="0">
         <v>150</v>
@@ -5846,7 +5884,7 @@
         <v>40</v>
       </c>
       <c r="L139" s="0">
-        <v>229.9799999999999</v>
+        <v>227.75499999999977</v>
       </c>
     </row>
     <row r="140">
@@ -5857,7 +5895,7 @@
         <v>110</v>
       </c>
       <c r="C140" s="0">
-        <v>58.839912289304074</v>
+        <v>59.820577494125814</v>
       </c>
       <c r="D140" s="0">
         <v>150</v>
@@ -5922,7 +5960,7 @@
         <v>40</v>
       </c>
       <c r="L141" s="0">
-        <v>232.34000000000003</v>
+        <v>227.93999999999983</v>
       </c>
     </row>
     <row r="142">
@@ -5933,7 +5971,7 @@
         <v>110</v>
       </c>
       <c r="C142" s="0">
-        <v>58.839912289304074</v>
+        <v>60.310910096536681</v>
       </c>
       <c r="D142" s="0">
         <v>150</v>
@@ -5998,7 +6036,7 @@
         <v>40</v>
       </c>
       <c r="L143" s="0">
-        <v>234.69999999999999</v>
+        <v>228.17500000000001</v>
       </c>
     </row>
     <row r="144">
@@ -6085,7 +6123,7 @@
         <v>110</v>
       </c>
       <c r="C146" s="0">
-        <v>60.801242698947547</v>
+        <v>61.291575301358414</v>
       </c>
       <c r="D146" s="0">
         <v>150</v>
@@ -6150,7 +6188,7 @@
         <v>40</v>
       </c>
       <c r="L147" s="0">
-        <v>230.54000000000019</v>
+        <v>228.31000000000017</v>
       </c>
     </row>
     <row r="148">
@@ -6161,7 +6199,7 @@
         <v>110</v>
       </c>
       <c r="C148" s="0">
-        <v>60.801242698947547</v>
+        <v>61.291575301358414</v>
       </c>
       <c r="D148" s="0">
         <v>150</v>
@@ -6226,7 +6264,7 @@
         <v>40</v>
       </c>
       <c r="L149" s="0">
-        <v>232.80999999999995</v>
+        <v>230.60249999999996</v>
       </c>
     </row>
     <row r="150">
@@ -6237,7 +6275,7 @@
         <v>110</v>
       </c>
       <c r="C150" s="0">
-        <v>60.801242698947547</v>
+        <v>61.78190790376928</v>
       </c>
       <c r="D150" s="0">
         <v>150</v>
@@ -6264,7 +6302,7 @@
         <v>100</v>
       </c>
       <c r="L150" s="0">
-        <v>402.43999999999994</v>
+        <v>402.44000000000005</v>
       </c>
     </row>
     <row r="151">
@@ -6302,7 +6340,7 @@
         <v>40</v>
       </c>
       <c r="L151" s="0">
-        <v>235.07999999999993</v>
+        <v>230.71000000000004</v>
       </c>
     </row>
     <row r="152">
@@ -6313,7 +6351,7 @@
         <v>110</v>
       </c>
       <c r="C152" s="0">
-        <v>60.801242698947547</v>
+        <v>62.272240506180147</v>
       </c>
       <c r="D152" s="0">
         <v>150</v>
@@ -6378,7 +6416,7 @@
         <v>40</v>
       </c>
       <c r="L153" s="0">
-        <v>237.35000000000014</v>
+        <v>230.86250000000001</v>
       </c>
     </row>
     <row r="154">
@@ -6454,7 +6492,7 @@
         <v>40</v>
       </c>
       <c r="L155" s="0">
-        <v>231.05999999999983</v>
+        <v>231.06000000000006</v>
       </c>
     </row>
     <row r="156">
@@ -6465,7 +6503,7 @@
         <v>110</v>
       </c>
       <c r="C156" s="0">
-        <v>62.762573108591013</v>
+        <v>63.25290571100188</v>
       </c>
       <c r="D156" s="0">
         <v>150</v>
@@ -6530,7 +6568,7 @@
         <v>40</v>
       </c>
       <c r="L157" s="0">
-        <v>233.41999999999996</v>
+        <v>231.22749999999985</v>
       </c>
     </row>
     <row r="158">
@@ -6541,7 +6579,7 @@
         <v>110</v>
       </c>
       <c r="C158" s="0">
-        <v>62.762573108591013</v>
+        <v>63.743238313412753</v>
       </c>
       <c r="D158" s="0">
         <v>150</v>
@@ -6568,7 +6606,7 @@
         <v>100</v>
       </c>
       <c r="L158" s="0">
-        <v>407.4799999999999</v>
+        <v>407.48000000000002</v>
       </c>
     </row>
     <row r="159">
@@ -6606,7 +6644,7 @@
         <v>40</v>
       </c>
       <c r="L159" s="0">
-        <v>235.77999999999986</v>
+        <v>231.43999999999994</v>
       </c>
     </row>
     <row r="160">
@@ -6617,7 +6655,7 @@
         <v>110</v>
       </c>
       <c r="C160" s="0">
-        <v>62.762573108591013</v>
+        <v>64.23357091582362</v>
       </c>
       <c r="D160" s="0">
         <v>150</v>
@@ -6682,7 +6720,7 @@
         <v>40</v>
       </c>
       <c r="L161" s="0">
-        <v>238.13999999999976</v>
+        <v>231.69749999999999</v>
       </c>
     </row>
     <row r="162">
@@ -6693,7 +6731,7 @@
         <v>110</v>
       </c>
       <c r="C162" s="0">
-        <v>62.762573108591013</v>
+        <v>64.23357091582362</v>
       </c>
       <c r="D162" s="0">
         <v>150</v>
@@ -6758,7 +6796,7 @@
         <v>40</v>
       </c>
       <c r="L163" s="0">
-        <v>240.5</v>
+        <v>234.125</v>
       </c>
     </row>
     <row r="164">
@@ -6845,7 +6883,7 @@
         <v>110</v>
       </c>
       <c r="C166" s="0">
-        <v>64.723903518234479</v>
+        <v>65</v>
       </c>
       <c r="D166" s="0">
         <v>150</v>
@@ -6872,7 +6910,7 @@
         <v>100</v>
       </c>
       <c r="L166" s="0">
-        <v>412.5200000000001</v>
+        <v>412.51999999999998</v>
       </c>
     </row>
     <row r="167">
@@ -6910,7 +6948,7 @@
         <v>40</v>
       </c>
       <c r="L167" s="0">
-        <v>236.51999999999998</v>
+        <v>234.36000000000013</v>
       </c>
     </row>
     <row r="168">
@@ -6921,7 +6959,7 @@
         <v>110</v>
       </c>
       <c r="C168" s="0">
-        <v>64.723903518234479</v>
+        <v>65</v>
       </c>
       <c r="D168" s="0">
         <v>150</v>
@@ -6986,7 +7024,7 @@
         <v>40</v>
       </c>
       <c r="L169" s="0">
-        <v>238.77999999999997</v>
+        <v>234.5</v>
       </c>
     </row>
     <row r="170">
@@ -6997,7 +7035,7 @@
         <v>110</v>
       </c>
       <c r="C170" s="0">
-        <v>64.723903518234479</v>
+        <v>65</v>
       </c>
       <c r="D170" s="0">
         <v>150</v>
@@ -7062,7 +7100,7 @@
         <v>40</v>
       </c>
       <c r="L171" s="0">
-        <v>241.03999999999996</v>
+        <v>234.67999999999984</v>
       </c>
     </row>
     <row r="172">
@@ -7176,7 +7214,7 @@
         <v>100</v>
       </c>
       <c r="L174" s="0">
-        <v>417.56000000000006</v>
+        <v>417.55999999999995</v>
       </c>
     </row>
     <row r="175">
@@ -7214,7 +7252,7 @@
         <v>40</v>
       </c>
       <c r="L175" s="0">
-        <v>237.24000000000001</v>
+        <v>235.09999999999991</v>
       </c>
     </row>
     <row r="176">
@@ -7290,7 +7328,7 @@
         <v>40</v>
       </c>
       <c r="L177" s="0">
-        <v>239.58000000000015</v>
+        <v>237.46250000000009</v>
       </c>
     </row>
     <row r="178">
@@ -7366,7 +7404,7 @@
         <v>40</v>
       </c>
       <c r="L179" s="0">
-        <v>241.92000000000007</v>
+        <v>237.73000000000002</v>
       </c>
     </row>
     <row r="180">
@@ -7442,7 +7480,7 @@
         <v>40</v>
       </c>
       <c r="L181" s="0">
-        <v>244.25999999999999</v>
+        <v>238.0424999999999</v>
       </c>
     </row>
     <row r="182">
@@ -7594,7 +7632,7 @@
         <v>40</v>
       </c>
       <c r="L185" s="0">
-        <v>240.6600000000002</v>
+        <v>240.65999999999997</v>
       </c>
     </row>
     <row r="186">
@@ -7670,7 +7708,7 @@
         <v>40</v>
       </c>
       <c r="L187" s="0">
-        <v>242.92000000000019</v>
+        <v>242.91999999999996</v>
       </c>
     </row>
     <row r="188">
@@ -7936,7 +7974,7 @@
         <v>100</v>
       </c>
       <c r="L194" s="0">
-        <v>430.04000000000008</v>
+        <v>430.03999999999996</v>
       </c>
     </row>
     <row r="195">
@@ -8012,7 +8050,7 @@
         <v>100</v>
       </c>
       <c r="L196" s="0">
-        <v>431.28000000000009</v>
+        <v>431.27999999999997</v>
       </c>
     </row>
     <row r="197">
@@ -8202,7 +8240,7 @@
         <v>40</v>
       </c>
       <c r="L201" s="0">
-        <v>258.74000000000012</v>
+        <v>258.7399999999999</v>
       </c>
     </row>
     <row r="202">
@@ -8468,7 +8506,7 @@
         <v>100</v>
       </c>
       <c r="L208" s="0">
-        <v>438.71999999999991</v>
+        <v>438.72000000000003</v>
       </c>
     </row>
     <row r="209">
@@ -8544,7 +8582,7 @@
         <v>100</v>
       </c>
       <c r="L210" s="0">
-        <v>439.95999999999992</v>
+        <v>439.96000000000004</v>
       </c>
     </row>
     <row r="211">
@@ -8582,7 +8620,7 @@
         <v>40</v>
       </c>
       <c r="L211" s="0">
-        <v>269.44000000000005</v>
+        <v>269.43999999999983</v>
       </c>
     </row>
     <row r="212">
@@ -8734,7 +8772,7 @@
         <v>40</v>
       </c>
       <c r="L215" s="0">
-        <v>273.66000000000008</v>
+        <v>273.65999999999985</v>
       </c>
     </row>
     <row r="216">
@@ -8772,7 +8810,7 @@
         <v>100</v>
       </c>
       <c r="L216" s="0">
-        <v>439.42000000000007</v>
+        <v>442.61499999999995</v>
       </c>
     </row>
     <row r="217">
@@ -8783,7 +8821,7 @@
         <v>55</v>
       </c>
       <c r="C217" s="0">
-        <v>11.767982457860816</v>
+        <v>10.296984650628213</v>
       </c>
       <c r="D217" s="0">
         <v>49.999999999999986</v>
@@ -8848,7 +8886,7 @@
         <v>100</v>
       </c>
       <c r="L218" s="0">
-        <v>440.67999999999995</v>
+        <v>443.85999999999996</v>
       </c>
     </row>
     <row r="219">
@@ -8859,7 +8897,7 @@
         <v>55</v>
       </c>
       <c r="C219" s="0">
-        <v>11.767982457860816</v>
+        <v>10.296984650628213</v>
       </c>
       <c r="D219" s="0">
         <v>49.999999999999986</v>
@@ -8924,7 +8962,7 @@
         <v>100</v>
       </c>
       <c r="L220" s="0">
-        <v>441.93999999999994</v>
+        <v>445.10499999999996</v>
       </c>
     </row>
     <row r="221">
@@ -8935,7 +8973,7 @@
         <v>55</v>
       </c>
       <c r="C221" s="0">
-        <v>11.767982457860816</v>
+        <v>10.296984650628213</v>
       </c>
       <c r="D221" s="0">
         <v>49.999999999999986</v>
@@ -8962,7 +9000,7 @@
         <v>40</v>
       </c>
       <c r="L221" s="0">
-        <v>279.99000000000001</v>
+        <v>279.98999999999978</v>
       </c>
     </row>
     <row r="222">
@@ -9000,7 +9038,7 @@
         <v>100</v>
       </c>
       <c r="L222" s="0">
-        <v>443.19999999999999</v>
+        <v>445.29999999999995</v>
       </c>
     </row>
     <row r="223">
@@ -9011,7 +9049,7 @@
         <v>55</v>
       </c>
       <c r="C223" s="0">
-        <v>11.767982457860816</v>
+        <v>10.787317253039081</v>
       </c>
       <c r="D223" s="0">
         <v>49.999999999999986</v>
@@ -9076,7 +9114,7 @@
         <v>100</v>
       </c>
       <c r="L224" s="0">
-        <v>444.44000000000011</v>
+        <v>446.53499999999997</v>
       </c>
     </row>
     <row r="225">
@@ -9087,7 +9125,7 @@
         <v>55</v>
       </c>
       <c r="C225" s="0">
-        <v>11.767982457860816</v>
+        <v>10.787317253039081</v>
       </c>
       <c r="D225" s="0">
         <v>49.999999999999986</v>
@@ -9152,7 +9190,7 @@
         <v>100</v>
       </c>
       <c r="L226" s="0">
-        <v>445.68000000000012</v>
+        <v>447.76999999999998</v>
       </c>
     </row>
     <row r="227">
@@ -9163,7 +9201,7 @@
         <v>55</v>
       </c>
       <c r="C227" s="0">
-        <v>11.767982457860816</v>
+        <v>10.787317253039081</v>
       </c>
       <c r="D227" s="0">
         <v>49.999999999999986</v>
@@ -9228,7 +9266,7 @@
         <v>100</v>
       </c>
       <c r="L228" s="0">
-        <v>446.92000000000002</v>
+        <v>447.96249999999998</v>
       </c>
     </row>
     <row r="229">
@@ -9239,7 +9277,7 @@
         <v>55</v>
       </c>
       <c r="C229" s="0">
-        <v>11.767982457860816</v>
+        <v>11.277649855449948</v>
       </c>
       <c r="D229" s="0">
         <v>49.999999999999986</v>
@@ -9304,7 +9342,7 @@
         <v>100</v>
       </c>
       <c r="L230" s="0">
-        <v>448.16000000000003</v>
+        <v>449.19999999999993</v>
       </c>
     </row>
     <row r="231">
@@ -9315,7 +9353,7 @@
         <v>55</v>
       </c>
       <c r="C231" s="0">
-        <v>11.767982457860816</v>
+        <v>11.277649855449948</v>
       </c>
       <c r="D231" s="0">
         <v>49.999999999999986</v>
@@ -9456,7 +9494,7 @@
         <v>100</v>
       </c>
       <c r="L234" s="0">
-        <v>450.64000000000004</v>
+        <v>450.64000000000016</v>
       </c>
     </row>
     <row r="235">
@@ -9532,7 +9570,7 @@
         <v>100</v>
       </c>
       <c r="L236" s="0">
-        <v>451.88000000000005</v>
+        <v>451.88000000000017</v>
       </c>
     </row>
     <row r="237">
@@ -9608,7 +9646,7 @@
         <v>100</v>
       </c>
       <c r="L238" s="0">
-        <v>448.32000000000005</v>
+        <v>451.92000000000007</v>
       </c>
     </row>
     <row r="239">
@@ -9619,7 +9657,7 @@
         <v>55</v>
       </c>
       <c r="C239" s="0">
-        <v>13.729312867504285</v>
+        <v>12.258315060271682</v>
       </c>
       <c r="D239" s="0">
         <v>49.999999999999986</v>
@@ -9684,7 +9722,7 @@
         <v>100</v>
       </c>
       <c r="L240" s="0">
-        <v>449.56000000000006</v>
+        <v>453.16000000000008</v>
       </c>
     </row>
     <row r="241">
@@ -9695,7 +9733,7 @@
         <v>55</v>
       </c>
       <c r="C241" s="0">
-        <v>13.729312867504285</v>
+        <v>12.258315060271682</v>
       </c>
       <c r="D241" s="0">
         <v>49.999999999999986</v>
@@ -9760,7 +9798,7 @@
         <v>100</v>
       </c>
       <c r="L242" s="0">
-        <v>450.80000000000001</v>
+        <v>454.40000000000003</v>
       </c>
     </row>
     <row r="243">
@@ -9771,7 +9809,7 @@
         <v>55</v>
       </c>
       <c r="C243" s="0">
-        <v>13.729312867504285</v>
+        <v>12.258315060271682</v>
       </c>
       <c r="D243" s="0">
         <v>49.999999999999986</v>
@@ -9836,7 +9874,7 @@
         <v>100</v>
       </c>
       <c r="L244" s="0">
-        <v>452.03000000000003</v>
+        <v>454.42000000000007</v>
       </c>
     </row>
     <row r="245">
@@ -9847,7 +9885,7 @@
         <v>55</v>
       </c>
       <c r="C245" s="0">
-        <v>13.729312867504285</v>
+        <v>12.748647662682551</v>
       </c>
       <c r="D245" s="0">
         <v>49.999999999999986</v>
@@ -9912,7 +9950,7 @@
         <v>100</v>
       </c>
       <c r="L246" s="0">
-        <v>453.26000000000005</v>
+        <v>455.6400000000001</v>
       </c>
     </row>
     <row r="247">
@@ -9923,7 +9961,7 @@
         <v>55</v>
       </c>
       <c r="C247" s="0">
-        <v>13.729312867504285</v>
+        <v>12.748647662682551</v>
       </c>
       <c r="D247" s="0">
         <v>49.999999999999986</v>
@@ -9988,7 +10026,7 @@
         <v>100</v>
       </c>
       <c r="L248" s="0">
-        <v>454.48999999999995</v>
+        <v>456.8599999999999</v>
       </c>
     </row>
     <row r="249">
@@ -9999,7 +10037,7 @@
         <v>55</v>
       </c>
       <c r="C249" s="0">
-        <v>13.729312867504285</v>
+        <v>12.748647662682551</v>
       </c>
       <c r="D249" s="0">
         <v>49.999999999999986</v>
@@ -10064,7 +10102,7 @@
         <v>100</v>
       </c>
       <c r="L250" s="0">
-        <v>455.71999999999997</v>
+        <v>456.89999999999998</v>
       </c>
     </row>
     <row r="251">
@@ -10075,7 +10113,7 @@
         <v>55</v>
       </c>
       <c r="C251" s="0">
-        <v>13.729312867504285</v>
+        <v>13.238980265093417</v>
       </c>
       <c r="D251" s="0">
         <v>49.999999999999986</v>
@@ -10140,7 +10178,7 @@
         <v>100</v>
       </c>
       <c r="L252" s="0">
-        <v>456.94999999999999</v>
+        <v>458.125</v>
       </c>
     </row>
     <row r="253">
@@ -10151,7 +10189,7 @@
         <v>55</v>
       </c>
       <c r="C253" s="0">
-        <v>13.729312867504285</v>
+        <v>13.238980265093417</v>
       </c>
       <c r="D253" s="0">
         <v>49.999999999999986</v>
@@ -10216,7 +10254,7 @@
         <v>100</v>
       </c>
       <c r="L254" s="0">
-        <v>458.18000000000001</v>
+        <v>459.35000000000002</v>
       </c>
     </row>
     <row r="255">
@@ -10227,7 +10265,7 @@
         <v>55</v>
       </c>
       <c r="C255" s="0">
-        <v>13.729312867504285</v>
+        <v>13.238980265093417</v>
       </c>
       <c r="D255" s="0">
         <v>49.999999999999986</v>
@@ -10444,7 +10482,7 @@
         <v>100</v>
       </c>
       <c r="L260" s="0">
-        <v>457.05999999999995</v>
+        <v>460.66750000000013</v>
       </c>
     </row>
     <row r="261">
@@ -10455,7 +10493,7 @@
         <v>55</v>
       </c>
       <c r="C261" s="0">
-        <v>15.690643277147753</v>
+        <v>14.219645469915152</v>
       </c>
       <c r="D261" s="0">
         <v>49.999999999999986</v>
@@ -10520,7 +10558,7 @@
         <v>100</v>
       </c>
       <c r="L262" s="0">
-        <v>458.30000000000001</v>
+        <v>461.90000000000003</v>
       </c>
     </row>
     <row r="263">
@@ -10531,7 +10569,7 @@
         <v>55</v>
       </c>
       <c r="C263" s="0">
-        <v>15.690643277147753</v>
+        <v>14.219645469915152</v>
       </c>
       <c r="D263" s="0">
         <v>49.999999999999986</v>
@@ -10596,7 +10634,7 @@
         <v>100</v>
       </c>
       <c r="L264" s="0">
-        <v>459.53000000000014</v>
+        <v>463.1225</v>
       </c>
     </row>
     <row r="265">
@@ -10607,7 +10645,7 @@
         <v>55</v>
       </c>
       <c r="C265" s="0">
-        <v>15.690643277147753</v>
+        <v>14.219645469915152</v>
       </c>
       <c r="D265" s="0">
         <v>49.999999999999986</v>
@@ -10672,7 +10710,7 @@
         <v>100</v>
       </c>
       <c r="L266" s="0">
-        <v>460.76000000000016</v>
+        <v>463.15000000000009</v>
       </c>
     </row>
     <row r="267">
@@ -10683,7 +10721,7 @@
         <v>55</v>
       </c>
       <c r="C267" s="0">
-        <v>15.690643277147753</v>
+        <v>14.709978072326019</v>
       </c>
       <c r="D267" s="0">
         <v>49.999999999999986</v>
@@ -10748,7 +10786,7 @@
         <v>100</v>
       </c>
       <c r="L268" s="0">
-        <v>461.99000000000007</v>
+        <v>464.375</v>
       </c>
     </row>
     <row r="269">
@@ -10759,7 +10797,7 @@
         <v>55</v>
       </c>
       <c r="C269" s="0">
-        <v>15.690643277147753</v>
+        <v>14.709978072326019</v>
       </c>
       <c r="D269" s="0">
         <v>49.999999999999986</v>
@@ -10824,7 +10862,7 @@
         <v>100</v>
       </c>
       <c r="L270" s="0">
-        <v>463.22000000000008</v>
+        <v>465.60000000000002</v>
       </c>
     </row>
     <row r="271">
@@ -10835,7 +10873,7 @@
         <v>55</v>
       </c>
       <c r="C271" s="0">
-        <v>15.690643277147753</v>
+        <v>14.709978072326019</v>
       </c>
       <c r="D271" s="0">
         <v>49.999999999999986</v>
@@ -10900,7 +10938,7 @@
         <v>100</v>
       </c>
       <c r="L272" s="0">
-        <v>464.4500000000001</v>
+        <v>465.63750000000005</v>
       </c>
     </row>
     <row r="273">
@@ -10911,7 +10949,7 @@
         <v>55</v>
       </c>
       <c r="C273" s="0">
-        <v>15.690643277147753</v>
+        <v>15.200310674736887</v>
       </c>
       <c r="D273" s="0">
         <v>49.999999999999986</v>
@@ -10976,7 +11014,7 @@
         <v>100</v>
       </c>
       <c r="L274" s="0">
-        <v>465.68000000000012</v>
+        <v>466.86500000000012</v>
       </c>
     </row>
     <row r="275">
@@ -10987,7 +11025,7 @@
         <v>55</v>
       </c>
       <c r="C275" s="0">
-        <v>15.690643277147753</v>
+        <v>15.200310674736887</v>
       </c>
       <c r="D275" s="0">
         <v>49.999999999999986</v>
@@ -11052,7 +11090,7 @@
         <v>100</v>
       </c>
       <c r="L276" s="0">
-        <v>466.91000000000014</v>
+        <v>468.09250000000009</v>
       </c>
     </row>
     <row r="277">
@@ -11063,7 +11101,7 @@
         <v>55</v>
       </c>
       <c r="C277" s="0">
-        <v>15.690643277147753</v>
+        <v>15.200310674736887</v>
       </c>
       <c r="D277" s="0">
         <v>49.999999999999986</v>
@@ -11128,7 +11166,7 @@
         <v>100</v>
       </c>
       <c r="L278" s="0">
-        <v>468.14000000000004</v>
+        <v>468.13999999999993</v>
       </c>
     </row>
     <row r="279">
@@ -11204,7 +11242,7 @@
         <v>100</v>
       </c>
       <c r="L280" s="0">
-        <v>469.37000000000006</v>
+        <v>469.36999999999995</v>
       </c>
     </row>
     <row r="281">
@@ -11356,7 +11394,7 @@
         <v>100</v>
       </c>
       <c r="L284" s="0">
-        <v>467.34000000000003</v>
+        <v>470.70749999999998</v>
       </c>
     </row>
     <row r="285">
@@ -11367,7 +11405,7 @@
         <v>55</v>
       </c>
       <c r="C285" s="0">
-        <v>17.651973686791223</v>
+        <v>16.18097587955862</v>
       </c>
       <c r="D285" s="0">
         <v>49.999999999999986</v>
@@ -11394,7 +11432,7 @@
         <v>40</v>
       </c>
       <c r="L285" s="0">
-        <v>341.4799999999999</v>
+        <v>341.48000000000002</v>
       </c>
     </row>
     <row r="286">
@@ -11432,7 +11470,7 @@
         <v>100</v>
       </c>
       <c r="L286" s="0">
-        <v>468.58000000000004</v>
+        <v>471.94000000000005</v>
       </c>
     </row>
     <row r="287">
@@ -11443,7 +11481,7 @@
         <v>55</v>
       </c>
       <c r="C287" s="0">
-        <v>17.651973686791223</v>
+        <v>16.18097587955862</v>
       </c>
       <c r="D287" s="0">
         <v>49.999999999999986</v>
@@ -11470,7 +11508,7 @@
         <v>40</v>
       </c>
       <c r="L287" s="0">
-        <v>343.25999999999999</v>
+        <v>343.2600000000001</v>
       </c>
     </row>
     <row r="288">
@@ -11508,7 +11546,7 @@
         <v>100</v>
       </c>
       <c r="L288" s="0">
-        <v>469.81999999999994</v>
+        <v>473.17250000000001</v>
       </c>
     </row>
     <row r="289">
@@ -11519,7 +11557,7 @@
         <v>55</v>
       </c>
       <c r="C289" s="0">
-        <v>17.651973686791223</v>
+        <v>16.18097587955862</v>
       </c>
       <c r="D289" s="0">
         <v>49.999999999999986</v>
@@ -11546,7 +11584,7 @@
         <v>40</v>
       </c>
       <c r="L289" s="0">
-        <v>345.03999999999985</v>
+        <v>345.03999999999996</v>
       </c>
     </row>
     <row r="290">
@@ -11584,7 +11622,7 @@
         <v>100</v>
       </c>
       <c r="L290" s="0">
-        <v>471.05999999999995</v>
+        <v>473.28999999999996</v>
       </c>
     </row>
     <row r="291">
@@ -11595,7 +11633,7 @@
         <v>55</v>
       </c>
       <c r="C291" s="0">
-        <v>17.651973686791223</v>
+        <v>16.67130848196949</v>
       </c>
       <c r="D291" s="0">
         <v>49.999999999999986</v>
@@ -11660,7 +11698,7 @@
         <v>100</v>
       </c>
       <c r="L292" s="0">
-        <v>472.30000000000007</v>
+        <v>474.52499999999998</v>
       </c>
     </row>
     <row r="293">
@@ -11671,7 +11709,7 @@
         <v>55</v>
       </c>
       <c r="C293" s="0">
-        <v>17.651973686791223</v>
+        <v>16.67130848196949</v>
       </c>
       <c r="D293" s="0">
         <v>49.999999999999986</v>
@@ -11736,7 +11774,7 @@
         <v>100</v>
       </c>
       <c r="L294" s="0">
-        <v>473.54000000000008</v>
+        <v>475.7600000000001</v>
       </c>
     </row>
     <row r="295">
@@ -11747,7 +11785,7 @@
         <v>55</v>
       </c>
       <c r="C295" s="0">
-        <v>17.651973686791223</v>
+        <v>16.67130848196949</v>
       </c>
       <c r="D295" s="0">
         <v>49.999999999999986</v>
@@ -11812,7 +11850,7 @@
         <v>100</v>
       </c>
       <c r="L296" s="0">
-        <v>474.78000000000009</v>
+        <v>475.88750000000005</v>
       </c>
     </row>
     <row r="297">
@@ -11823,7 +11861,7 @@
         <v>55</v>
       </c>
       <c r="C297" s="0">
-        <v>17.651973686791223</v>
+        <v>17.161641084380356</v>
       </c>
       <c r="D297" s="0">
         <v>49.999999999999986</v>
@@ -11888,7 +11926,7 @@
         <v>100</v>
       </c>
       <c r="L298" s="0">
-        <v>476.01999999999998</v>
+        <v>477.125</v>
       </c>
     </row>
     <row r="299">
@@ -11899,7 +11937,7 @@
         <v>55</v>
       </c>
       <c r="C299" s="0">
-        <v>17.651973686791223</v>
+        <v>17.161641084380356</v>
       </c>
       <c r="D299" s="0">
         <v>49.999999999999986</v>
@@ -12192,7 +12230,7 @@
         <v>100</v>
       </c>
       <c r="L306" s="0">
-        <v>476.58000000000004</v>
+        <v>479.85000000000002</v>
       </c>
     </row>
     <row r="307">
@@ -12203,7 +12241,7 @@
         <v>55</v>
       </c>
       <c r="C307" s="0">
-        <v>19.613304096434693</v>
+        <v>18.142306289202089</v>
       </c>
       <c r="D307" s="0">
         <v>49.999999999999986</v>
@@ -12268,7 +12306,7 @@
         <v>100</v>
       </c>
       <c r="L308" s="0">
-        <v>477.81999999999994</v>
+        <v>481.07499999999993</v>
       </c>
     </row>
     <row r="309">
@@ -12279,7 +12317,7 @@
         <v>55</v>
       </c>
       <c r="C309" s="0">
-        <v>19.613304096434693</v>
+        <v>18.142306289202089</v>
       </c>
       <c r="D309" s="0">
         <v>49.999999999999986</v>
@@ -12344,7 +12382,7 @@
         <v>100</v>
       </c>
       <c r="L310" s="0">
-        <v>479.05999999999995</v>
+        <v>482.29999999999995</v>
       </c>
     </row>
     <row r="311">
@@ -12355,7 +12393,7 @@
         <v>55</v>
       </c>
       <c r="C311" s="0">
-        <v>19.613304096434693</v>
+        <v>18.142306289202089</v>
       </c>
       <c r="D311" s="0">
         <v>49.999999999999986</v>
@@ -12420,7 +12458,7 @@
         <v>100</v>
       </c>
       <c r="L312" s="0">
-        <v>480.29999999999995</v>
+        <v>482.45000000000005</v>
       </c>
     </row>
     <row r="313">
@@ -12431,7 +12469,7 @@
         <v>55</v>
       </c>
       <c r="C313" s="0">
-        <v>19.613304096434693</v>
+        <v>18.632638891612956</v>
       </c>
       <c r="D313" s="0">
         <v>49.999999999999986</v>
@@ -12496,7 +12534,7 @@
         <v>100</v>
       </c>
       <c r="L314" s="0">
-        <v>481.54000000000008</v>
+        <v>483.68000000000006</v>
       </c>
     </row>
     <row r="315">
@@ -12507,7 +12545,7 @@
         <v>55</v>
       </c>
       <c r="C315" s="0">
-        <v>19.613304096434693</v>
+        <v>18.632638891612956</v>
       </c>
       <c r="D315" s="0">
         <v>49.999999999999986</v>
@@ -12534,7 +12572,7 @@
         <v>40</v>
       </c>
       <c r="L315" s="0">
-        <v>367.75999999999999</v>
+        <v>367.7600000000001</v>
       </c>
     </row>
     <row r="316">
@@ -12572,7 +12610,7 @@
         <v>100</v>
       </c>
       <c r="L316" s="0">
-        <v>482.78000000000009</v>
+        <v>483.84500000000003</v>
       </c>
     </row>
     <row r="317">
@@ -12583,7 +12621,7 @@
         <v>55</v>
       </c>
       <c r="C317" s="0">
-        <v>19.613304096434693</v>
+        <v>19.122971494023826</v>
       </c>
       <c r="D317" s="0">
         <v>49.999999999999986</v>
@@ -12610,7 +12648,7 @@
         <v>40</v>
       </c>
       <c r="L317" s="0">
-        <v>369.47000000000003</v>
+        <v>369.47000000000014</v>
       </c>
     </row>
     <row r="318">
@@ -12648,7 +12686,7 @@
         <v>100</v>
       </c>
       <c r="L318" s="0">
-        <v>484.01999999999998</v>
+        <v>485.07999999999993</v>
       </c>
     </row>
     <row r="319">
@@ -12659,7 +12697,7 @@
         <v>55</v>
       </c>
       <c r="C319" s="0">
-        <v>19.613304096434693</v>
+        <v>19.122971494023826</v>
       </c>
       <c r="D319" s="0">
         <v>49.999999999999986</v>
@@ -12724,7 +12762,7 @@
         <v>100</v>
       </c>
       <c r="L320" s="0">
-        <v>485.25999999999999</v>
+        <v>486.31499999999994</v>
       </c>
     </row>
     <row r="321">
@@ -12735,7 +12773,7 @@
         <v>55</v>
       </c>
       <c r="C321" s="0">
-        <v>19.613304096434693</v>
+        <v>19.122971494023826</v>
       </c>
       <c r="D321" s="0">
         <v>49.999999999999986</v>
@@ -12952,7 +12990,7 @@
         <v>100</v>
       </c>
       <c r="L326" s="0">
-        <v>484.78000000000003</v>
+        <v>487.90000000000003</v>
       </c>
     </row>
     <row r="327">
@@ -12963,7 +13001,7 @@
         <v>55</v>
       </c>
       <c r="C327" s="0">
-        <v>21.574634506078162</v>
+        <v>20.103636698845559</v>
       </c>
       <c r="D327" s="0">
         <v>49.999999999999986</v>
@@ -13028,7 +13066,7 @@
         <v>100</v>
       </c>
       <c r="L328" s="0">
-        <v>486.01999999999992</v>
+        <v>489.12499999999994</v>
       </c>
     </row>
     <row r="329">
@@ -13039,7 +13077,7 @@
         <v>55</v>
       </c>
       <c r="C329" s="0">
-        <v>21.574634506078162</v>
+        <v>20.103636698845559</v>
       </c>
       <c r="D329" s="0">
         <v>49.999999999999986</v>
@@ -13104,7 +13142,7 @@
         <v>100</v>
       </c>
       <c r="L330" s="0">
-        <v>487.26000000000005</v>
+        <v>490.35000000000008</v>
       </c>
     </row>
     <row r="331">
@@ -13115,7 +13153,7 @@
         <v>55</v>
       </c>
       <c r="C331" s="0">
-        <v>21.574634506078162</v>
+        <v>20.103636698845559</v>
       </c>
       <c r="D331" s="0">
         <v>49.999999999999986</v>
@@ -13180,7 +13218,7 @@
         <v>100</v>
       </c>
       <c r="L332" s="0">
-        <v>488.50000000000006</v>
+        <v>490.55000000000001</v>
       </c>
     </row>
     <row r="333">
@@ -13191,7 +13229,7 @@
         <v>55</v>
       </c>
       <c r="C333" s="0">
-        <v>21.574634506078162</v>
+        <v>20.593969301256426</v>
       </c>
       <c r="D333" s="0">
         <v>49.999999999999986</v>
@@ -13256,7 +13294,7 @@
         <v>100</v>
       </c>
       <c r="L334" s="0">
-        <v>489.74000000000007</v>
+        <v>491.78000000000003</v>
       </c>
     </row>
     <row r="335">
@@ -13267,7 +13305,7 @@
         <v>55</v>
       </c>
       <c r="C335" s="0">
-        <v>21.574634506078162</v>
+        <v>20.593969301256426</v>
       </c>
       <c r="D335" s="0">
         <v>49.999999999999986</v>
@@ -13294,7 +13332,7 @@
         <v>40</v>
       </c>
       <c r="L335" s="0">
-        <v>384.62</v>
+        <v>384.62000000000012</v>
       </c>
     </row>
     <row r="336">
@@ -13332,7 +13370,7 @@
         <v>100</v>
       </c>
       <c r="L336" s="0">
-        <v>490.98000000000008</v>
+        <v>491.99500000000018</v>
       </c>
     </row>
     <row r="337">
@@ -13343,7 +13381,7 @@
         <v>55</v>
       </c>
       <c r="C337" s="0">
-        <v>21.574634506078162</v>
+        <v>21.084301903667296</v>
       </c>
       <c r="D337" s="0">
         <v>49.999999999999986</v>
@@ -13370,7 +13408,7 @@
         <v>40</v>
       </c>
       <c r="L337" s="0">
-        <v>386.29000000000008</v>
+        <v>386.29000000000019</v>
       </c>
     </row>
     <row r="338">
@@ -13408,7 +13446,7 @@
         <v>100</v>
       </c>
       <c r="L338" s="0">
-        <v>492.21999999999997</v>
+        <v>493.23000000000008</v>
       </c>
     </row>
     <row r="339">
@@ -13419,7 +13457,7 @@
         <v>55</v>
       </c>
       <c r="C339" s="0">
-        <v>21.574634506078162</v>
+        <v>21.084301903667296</v>
       </c>
       <c r="D339" s="0">
         <v>49.999999999999986</v>
@@ -13446,7 +13484,7 @@
         <v>40</v>
       </c>
       <c r="L339" s="0">
-        <v>387.95999999999992</v>
+        <v>387.96000000000004</v>
       </c>
     </row>
     <row r="340">
@@ -13484,7 +13522,7 @@
         <v>100</v>
       </c>
       <c r="L340" s="0">
-        <v>493.46000000000009</v>
+        <v>494.4650000000002</v>
       </c>
     </row>
     <row r="341">
@@ -13495,7 +13533,7 @@
         <v>55</v>
       </c>
       <c r="C341" s="0">
-        <v>21.574634506078162</v>
+        <v>21.084301903667296</v>
       </c>
       <c r="D341" s="0">
         <v>49.999999999999986</v>
@@ -13522,7 +13560,7 @@
         <v>40</v>
       </c>
       <c r="L341" s="0">
-        <v>389.63000000000011</v>
+        <v>389.63000000000022</v>
       </c>
     </row>
     <row r="342">
@@ -13636,7 +13674,7 @@
         <v>100</v>
       </c>
       <c r="L344" s="0">
-        <v>495.93000000000012</v>
+        <v>495.93000000000001</v>
       </c>
     </row>
     <row r="345">
@@ -13712,7 +13750,7 @@
         <v>100</v>
       </c>
       <c r="L346" s="0">
-        <v>493.08000000000004</v>
+        <v>496.14000000000004</v>
       </c>
     </row>
     <row r="347">
@@ -13723,7 +13761,7 @@
         <v>55</v>
       </c>
       <c r="C347" s="0">
-        <v>23.535964915721632</v>
+        <v>22.064967108489029</v>
       </c>
       <c r="D347" s="0">
         <v>49.999999999999986</v>
@@ -13788,7 +13826,7 @@
         <v>100</v>
       </c>
       <c r="L348" s="0">
-        <v>494.31999999999994</v>
+        <v>497.3725</v>
       </c>
     </row>
     <row r="349">
@@ -13799,7 +13837,7 @@
         <v>55</v>
       </c>
       <c r="C349" s="0">
-        <v>23.535964915721632</v>
+        <v>22.064967108489029</v>
       </c>
       <c r="D349" s="0">
         <v>49.999999999999986</v>
@@ -13864,7 +13902,7 @@
         <v>100</v>
       </c>
       <c r="L350" s="0">
-        <v>495.56000000000006</v>
+        <v>497.59000000000015</v>
       </c>
     </row>
     <row r="351">
@@ -13875,7 +13913,7 @@
         <v>55</v>
       </c>
       <c r="C351" s="0">
-        <v>23.535964915721632</v>
+        <v>22.555299710899895</v>
       </c>
       <c r="D351" s="0">
         <v>49.999999999999986</v>
@@ -13940,7 +13978,7 @@
         <v>100</v>
       </c>
       <c r="L352" s="0">
-        <v>496.79999999999995</v>
+        <v>498.82500000000005</v>
       </c>
     </row>
     <row r="353">
@@ -13951,7 +13989,7 @@
         <v>55</v>
       </c>
       <c r="C353" s="0">
-        <v>23.535964915721632</v>
+        <v>22.555299710899895</v>
       </c>
       <c r="D353" s="0">
         <v>49.999999999999986</v>
@@ -14016,7 +14054,7 @@
         <v>100</v>
       </c>
       <c r="L354" s="0">
-        <v>498.04000000000008</v>
+        <v>500.06000000000006</v>
       </c>
     </row>
     <row r="355">
@@ -14027,7 +14065,7 @@
         <v>55</v>
       </c>
       <c r="C355" s="0">
-        <v>23.535964915721632</v>
+        <v>22.555299710899895</v>
       </c>
       <c r="D355" s="0">
         <v>49.999999999999986</v>
@@ -14092,7 +14130,7 @@
         <v>100</v>
       </c>
       <c r="L356" s="0">
-        <v>499.28000000000009</v>
+        <v>500.28750000000002</v>
       </c>
     </row>
     <row r="357">
@@ -14103,7 +14141,7 @@
         <v>55</v>
       </c>
       <c r="C357" s="0">
-        <v>23.535964915721632</v>
+        <v>23.045632313310762</v>
       </c>
       <c r="D357" s="0">
         <v>49.999999999999986</v>
@@ -14168,7 +14206,7 @@
         <v>100</v>
       </c>
       <c r="L358" s="0">
-        <v>500.51999999999998</v>
+        <v>501.52499999999998</v>
       </c>
     </row>
     <row r="359">
@@ -14179,7 +14217,7 @@
         <v>55</v>
       </c>
       <c r="C359" s="0">
-        <v>23.535964915721632</v>
+        <v>23.045632313310762</v>
       </c>
       <c r="D359" s="0">
         <v>49.999999999999986</v>
@@ -14472,7 +14510,7 @@
         <v>100</v>
       </c>
       <c r="L366" s="0">
-        <v>501.60000000000002</v>
+        <v>504.495</v>
       </c>
     </row>
     <row r="367">
@@ -14483,7 +14521,7 @@
         <v>55</v>
       </c>
       <c r="C367" s="0">
-        <v>25.497295325365101</v>
+        <v>24.026297518132498</v>
       </c>
       <c r="D367" s="0">
         <v>49.999999999999986</v>
@@ -14548,7 +14586,7 @@
         <v>100</v>
       </c>
       <c r="L368" s="0">
-        <v>502.85000000000002</v>
+        <v>505.7299999999999</v>
       </c>
     </row>
     <row r="369">
@@ -14559,7 +14597,7 @@
         <v>55</v>
       </c>
       <c r="C369" s="0">
-        <v>25.497295325365101</v>
+        <v>24.026297518132498</v>
       </c>
       <c r="D369" s="0">
         <v>49.999999999999986</v>
@@ -14586,7 +14624,7 @@
         <v>40</v>
       </c>
       <c r="L369" s="0">
-        <v>412.13999999999999</v>
+        <v>412.13999999999987</v>
       </c>
     </row>
     <row r="370">
@@ -14624,7 +14662,7 @@
         <v>100</v>
       </c>
       <c r="L370" s="0">
-        <v>504.10000000000014</v>
+        <v>506.01000000000005</v>
       </c>
     </row>
     <row r="371">
@@ -14635,7 +14673,7 @@
         <v>55</v>
       </c>
       <c r="C371" s="0">
-        <v>25.497295325365101</v>
+        <v>24.516630120543365</v>
       </c>
       <c r="D371" s="0">
         <v>49.999999999999986</v>
@@ -14700,7 +14738,7 @@
         <v>100</v>
       </c>
       <c r="L372" s="0">
-        <v>505.35000000000002</v>
+        <v>507.25</v>
       </c>
     </row>
     <row r="373">
@@ -14711,7 +14749,7 @@
         <v>55</v>
       </c>
       <c r="C373" s="0">
-        <v>25.497295325365101</v>
+        <v>24.516630120543365</v>
       </c>
       <c r="D373" s="0">
         <v>49.999999999999986</v>
@@ -14776,7 +14814,7 @@
         <v>100</v>
       </c>
       <c r="L374" s="0">
-        <v>506.60000000000002</v>
+        <v>507.54500000000007</v>
       </c>
     </row>
     <row r="375">
@@ -14787,7 +14825,7 @@
         <v>55</v>
       </c>
       <c r="C375" s="0">
-        <v>25.497295325365101</v>
+        <v>25.006962722954231</v>
       </c>
       <c r="D375" s="0">
         <v>49.999999999999986</v>
@@ -14814,7 +14852,7 @@
         <v>40</v>
       </c>
       <c r="L375" s="0">
-        <v>416.88</v>
+        <v>416.87999999999988</v>
       </c>
     </row>
     <row r="376">
@@ -14852,7 +14890,7 @@
         <v>100</v>
       </c>
       <c r="L376" s="0">
-        <v>507.85000000000002</v>
+        <v>508.79000000000008</v>
       </c>
     </row>
     <row r="377">
@@ -14863,7 +14901,7 @@
         <v>55</v>
       </c>
       <c r="C377" s="0">
-        <v>25.497295325365101</v>
+        <v>25.006962722954231</v>
       </c>
       <c r="D377" s="0">
         <v>49.999999999999986</v>
@@ -14890,7 +14928,7 @@
         <v>40</v>
       </c>
       <c r="L377" s="0">
-        <v>418.46000000000004</v>
+        <v>418.45999999999992</v>
       </c>
     </row>
     <row r="378">
@@ -14966,7 +15004,7 @@
         <v>40</v>
       </c>
       <c r="L379" s="0">
-        <v>420.03999999999996</v>
+        <v>420.03999999999985</v>
       </c>
     </row>
     <row r="380">
@@ -15042,7 +15080,7 @@
         <v>40</v>
       </c>
       <c r="L381" s="0">
-        <v>421.62000000000012</v>
+        <v>421.62</v>
       </c>
     </row>
     <row r="382">
@@ -15080,7 +15118,7 @@
         <v>100</v>
       </c>
       <c r="L382" s="0">
-        <v>507.80000000000001</v>
+        <v>510.65000000000009</v>
       </c>
     </row>
     <row r="383">
@@ -15091,7 +15129,7 @@
         <v>55</v>
       </c>
       <c r="C383" s="0">
-        <v>27.458625735008571</v>
+        <v>25.987627927775968</v>
       </c>
       <c r="D383" s="0">
         <v>49.999999999999986</v>
@@ -15156,7 +15194,7 @@
         <v>100</v>
       </c>
       <c r="L384" s="0">
-        <v>509.04000000000013</v>
+        <v>511.88250000000005</v>
       </c>
     </row>
     <row r="385">
@@ -15167,7 +15205,7 @@
         <v>55</v>
       </c>
       <c r="C385" s="0">
-        <v>27.458625735008571</v>
+        <v>25.987627927775968</v>
       </c>
       <c r="D385" s="0">
         <v>49.999999999999986</v>
@@ -15232,7 +15270,7 @@
         <v>100</v>
       </c>
       <c r="L386" s="0">
-        <v>510.28000000000014</v>
+        <v>512.17000000000007</v>
       </c>
     </row>
     <row r="387">
@@ -15243,7 +15281,7 @@
         <v>55</v>
       </c>
       <c r="C387" s="0">
-        <v>27.458625735008571</v>
+        <v>26.477960530186834</v>
       </c>
       <c r="D387" s="0">
         <v>49.999999999999986</v>
@@ -15270,7 +15308,7 @@
         <v>40</v>
       </c>
       <c r="L387" s="0">
-        <v>426.25999999999993</v>
+        <v>426.26000000000005</v>
       </c>
     </row>
     <row r="388">
@@ -15308,7 +15346,7 @@
         <v>100</v>
       </c>
       <c r="L388" s="0">
-        <v>511.52000000000004</v>
+        <v>513.40499999999997</v>
       </c>
     </row>
     <row r="389">
@@ -15319,7 +15357,7 @@
         <v>55</v>
       </c>
       <c r="C389" s="0">
-        <v>27.458625735008571</v>
+        <v>26.477960530186834</v>
       </c>
       <c r="D389" s="0">
         <v>49.999999999999986</v>
@@ -15384,7 +15422,7 @@
         <v>100</v>
       </c>
       <c r="L390" s="0">
-        <v>512.76000000000022</v>
+        <v>514.6400000000001</v>
       </c>
     </row>
     <row r="391">
@@ -15395,7 +15433,7 @@
         <v>55</v>
       </c>
       <c r="C391" s="0">
-        <v>27.458625735008571</v>
+        <v>26.477960530186834</v>
       </c>
       <c r="D391" s="0">
         <v>49.999999999999986</v>
@@ -15422,7 +15460,7 @@
         <v>40</v>
       </c>
       <c r="L391" s="0">
-        <v>429.31999999999999</v>
+        <v>429.32000000000011</v>
       </c>
     </row>
     <row r="392">
@@ -15460,7 +15498,7 @@
         <v>100</v>
       </c>
       <c r="L392" s="0">
-        <v>514</v>
+        <v>514.9375</v>
       </c>
     </row>
     <row r="393">
@@ -15471,7 +15509,7 @@
         <v>55</v>
       </c>
       <c r="C393" s="0">
-        <v>27.458625735008571</v>
+        <v>26.968293132597701</v>
       </c>
       <c r="D393" s="0">
         <v>49.999999999999986</v>
@@ -15536,7 +15574,7 @@
         <v>100</v>
       </c>
       <c r="L394" s="0">
-        <v>515.24000000000001</v>
+        <v>516.17500000000007</v>
       </c>
     </row>
     <row r="395">
@@ -15547,7 +15585,7 @@
         <v>55</v>
       </c>
       <c r="C395" s="0">
-        <v>27.458625735008571</v>
+        <v>26.968293132597701</v>
       </c>
       <c r="D395" s="0">
         <v>49.999999999999986</v>
@@ -15574,7 +15612,7 @@
         <v>40</v>
       </c>
       <c r="L395" s="0">
-        <v>432.37999999999994</v>
+        <v>432.38000000000005</v>
       </c>
     </row>
     <row r="396">
@@ -15726,7 +15764,7 @@
         <v>40</v>
       </c>
       <c r="L399" s="0">
-        <v>435.43999999999988</v>
+        <v>435.44</v>
       </c>
     </row>
     <row r="400">
@@ -15764,7 +15802,7 @@
         <v>100</v>
       </c>
       <c r="L400" s="0">
-        <v>515.15000000000009</v>
+        <v>518.00750000000005</v>
       </c>
     </row>
     <row r="401">
@@ -15775,7 +15813,7 @@
         <v>55</v>
       </c>
       <c r="C401" s="0">
-        <v>29.419956144652037</v>
+        <v>27.948958337419437</v>
       </c>
       <c r="D401" s="0">
         <v>49.999999999999986</v>
@@ -15840,7 +15878,7 @@
         <v>100</v>
       </c>
       <c r="L402" s="0">
-        <v>516.39999999999998</v>
+        <v>519.25</v>
       </c>
     </row>
     <row r="403">
@@ -15851,7 +15889,7 @@
         <v>55</v>
       </c>
       <c r="C403" s="0">
-        <v>29.419956144652037</v>
+        <v>27.948958337419437</v>
       </c>
       <c r="D403" s="0">
         <v>49.999999999999986</v>

</xml_diff>